<commit_message>
Version 0.2.5.5 Better xlsx
</commit_message>
<xml_diff>
--- a/data/Resultados.2024-09-07.xlsx
+++ b/data/Resultados.2024-09-07.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Resultados" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,13 +28,23 @@
     <font>
       <b val="1"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004F81BD"/>
+        <bgColor rgb="004F81BD"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,10 +65,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -134,6 +151,17 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Resultados" displayName="Resultados" ref="A1:B104" headerRowCount="1">
+  <autoFilter ref="A1:B104"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Jugador"/>
+    <tableColumn id="2" name="Puntos"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -420,7 +448,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -432,1050 +460,1056 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Jugador</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Puntos</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>KIM</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="4" t="n">
         <v>143</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>OSMANY</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="4" t="n">
         <v>120</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>DORIS</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="4" t="n">
         <v>114</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>CHAYO</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" s="4" t="n">
         <v>112</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="3" t="inlineStr">
         <is>
           <t>YENNIFER</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" s="4" t="n">
         <v>102</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="3" t="inlineStr">
         <is>
           <t>LUISANA ROMERO</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" s="4" t="n">
         <v>98</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="3" t="inlineStr">
         <is>
           <t>ALEC</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" s="4" t="n">
         <v>90</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="3" t="inlineStr">
         <is>
           <t>NATASHA</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B9" s="4" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="3" t="inlineStr">
         <is>
           <t>MAIRA TORRES</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="B10" s="4" t="n">
         <v>86</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="3" t="inlineStr">
         <is>
           <t>CHRISTIAN BUSTAMANTE</t>
         </is>
       </c>
-      <c r="B11" t="n">
+      <c r="B11" s="4" t="n">
         <v>85</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="3" t="inlineStr">
         <is>
           <t>GEORGINA RIZZO</t>
         </is>
       </c>
-      <c r="B12" t="n">
+      <c r="B12" s="4" t="n">
         <v>83</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="3" t="inlineStr">
         <is>
           <t>ANGELICA CHAVEZ</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="B13" s="4" t="n">
         <v>82</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="3" t="inlineStr">
         <is>
           <t>JENIFER PAOLA</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="B14" s="4" t="n">
         <v>82</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="3" t="inlineStr">
         <is>
           <t>SAMMY</t>
         </is>
       </c>
-      <c r="B15" t="n">
+      <c r="B15" s="4" t="n">
         <v>79</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="3" t="inlineStr">
         <is>
           <t>AHSLIN GIRON</t>
         </is>
       </c>
-      <c r="B16" t="n">
+      <c r="B16" s="4" t="n">
         <v>79</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="3" t="inlineStr">
         <is>
           <t>BLANKY RUIZ</t>
         </is>
       </c>
-      <c r="B17" t="n">
+      <c r="B17" s="4" t="n">
         <v>78</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="3" t="inlineStr">
         <is>
           <t>YANE</t>
         </is>
       </c>
-      <c r="B18" t="n">
+      <c r="B18" s="4" t="n">
         <v>78</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="3" t="inlineStr">
         <is>
           <t>YISETH</t>
         </is>
       </c>
-      <c r="B19" t="n">
+      <c r="B19" s="4" t="n">
         <v>78</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" s="3" t="inlineStr">
         <is>
           <t>HILLARY NICHOLE</t>
         </is>
       </c>
-      <c r="B20" t="n">
+      <c r="B20" s="4" t="n">
         <v>78</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" s="3" t="inlineStr">
         <is>
           <t>MARIE KREATIONS</t>
         </is>
       </c>
-      <c r="B21" t="n">
+      <c r="B21" s="4" t="n">
         <v>76</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" s="3" t="inlineStr">
         <is>
           <t>LEIDIMAR</t>
         </is>
       </c>
-      <c r="B22" t="n">
+      <c r="B22" s="4" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="3" t="inlineStr">
         <is>
           <t>PAUSINI</t>
         </is>
       </c>
-      <c r="B23" t="n">
+      <c r="B23" s="4" t="n">
         <v>73</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" s="3" t="inlineStr">
         <is>
           <t>DAYANA</t>
         </is>
       </c>
-      <c r="B24" t="n">
+      <c r="B24" s="4" t="n">
         <v>71</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" s="3" t="inlineStr">
         <is>
           <t>MARITZA</t>
         </is>
       </c>
-      <c r="B25" t="n">
+      <c r="B25" s="4" t="n">
         <v>70</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" s="3" t="inlineStr">
         <is>
           <t>ROSS</t>
         </is>
       </c>
-      <c r="B26" t="n">
+      <c r="B26" s="4" t="n">
         <v>69</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" s="3" t="inlineStr">
         <is>
           <t>BUENO</t>
         </is>
       </c>
-      <c r="B27" t="n">
+      <c r="B27" s="4" t="n">
         <v>69</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" s="3" t="inlineStr">
         <is>
           <t>XIMENA CAMACHO</t>
         </is>
       </c>
-      <c r="B28" t="n">
+      <c r="B28" s="4" t="n">
         <v>67</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" s="3" t="inlineStr">
         <is>
           <t>ANDREA TALAMANTE</t>
         </is>
       </c>
-      <c r="B29" t="n">
+      <c r="B29" s="4" t="n">
         <v>66</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" s="3" t="inlineStr">
         <is>
           <t>LIZ BRAVO</t>
         </is>
       </c>
-      <c r="B30" t="n">
+      <c r="B30" s="4" t="n">
         <v>65</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
+      <c r="A31" s="3" t="inlineStr">
         <is>
           <t>INEZ</t>
         </is>
       </c>
-      <c r="B31" t="n">
+      <c r="B31" s="4" t="n">
         <v>65</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A32" s="3" t="inlineStr">
         <is>
           <t>SUN</t>
         </is>
       </c>
-      <c r="B32" t="n">
+      <c r="B32" s="4" t="n">
         <v>65</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="A33" s="3" t="inlineStr">
         <is>
           <t>HEIMY</t>
         </is>
       </c>
-      <c r="B33" t="n">
+      <c r="B33" s="4" t="n">
         <v>64</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
+      <c r="A34" s="3" t="inlineStr">
         <is>
           <t>MAURA OCHOA</t>
         </is>
       </c>
-      <c r="B34" t="n">
+      <c r="B34" s="4" t="n">
         <v>62</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
+      <c r="A35" s="3" t="inlineStr">
         <is>
           <t>ANDREA</t>
         </is>
       </c>
-      <c r="B35" t="n">
+      <c r="B35" s="4" t="n">
         <v>60</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="A36" s="3" t="inlineStr">
         <is>
           <t>ALEXANDRA MARTINEZ</t>
         </is>
       </c>
-      <c r="B36" t="n">
+      <c r="B36" s="4" t="n">
         <v>60</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="A37" s="3" t="inlineStr">
         <is>
           <t>ALMA</t>
         </is>
       </c>
-      <c r="B37" t="n">
+      <c r="B37" s="4" t="n">
         <v>58</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="A38" s="3" t="inlineStr">
         <is>
           <t>KARINA</t>
         </is>
       </c>
-      <c r="B38" t="n">
+      <c r="B38" s="4" t="n">
         <v>54</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="A39" s="3" t="inlineStr">
         <is>
           <t>GLENDY</t>
         </is>
       </c>
-      <c r="B39" t="n">
+      <c r="B39" s="4" t="n">
         <v>45</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
+      <c r="A40" s="3" t="inlineStr">
         <is>
           <t>ROCIO GIANOLINI</t>
         </is>
       </c>
-      <c r="B40" t="n">
+      <c r="B40" s="4" t="n">
         <v>45</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
+      <c r="A41" s="3" t="inlineStr">
         <is>
           <t>YADI</t>
         </is>
       </c>
-      <c r="B41" t="n">
+      <c r="B41" s="4" t="n">
         <v>42</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
+      <c r="A42" s="3" t="inlineStr">
         <is>
           <t>NOHELIA</t>
         </is>
       </c>
-      <c r="B42" t="n">
+      <c r="B42" s="4" t="n">
         <v>41</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
+      <c r="A43" s="3" t="inlineStr">
         <is>
           <t>DENISSE VALENZUELA</t>
         </is>
       </c>
-      <c r="B43" t="n">
+      <c r="B43" s="4" t="n">
         <v>36</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
+      <c r="A44" s="3" t="inlineStr">
         <is>
           <t>JOHANNA RC</t>
         </is>
       </c>
-      <c r="B44" t="n">
+      <c r="B44" s="4" t="n">
         <v>36</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
+      <c r="A45" s="3" t="inlineStr">
         <is>
           <t>AURIS SALAS</t>
         </is>
       </c>
-      <c r="B45" t="n">
+      <c r="B45" s="4" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
+      <c r="A46" s="3" t="inlineStr">
         <is>
           <t>BRIANYS ORTIZ</t>
         </is>
       </c>
-      <c r="B46" t="n">
+      <c r="B46" s="4" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
+      <c r="A47" s="3" t="inlineStr">
         <is>
           <t>RUBI PERALTA</t>
         </is>
       </c>
-      <c r="B47" t="n">
+      <c r="B47" s="4" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
+      <c r="A48" s="3" t="inlineStr">
         <is>
           <t>DIANA</t>
         </is>
       </c>
-      <c r="B48" t="n">
+      <c r="B48" s="4" t="n">
         <v>31</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
+      <c r="A49" s="3" t="inlineStr">
         <is>
           <t>KEY</t>
         </is>
       </c>
-      <c r="B49" t="n">
+      <c r="B49" s="4" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
+      <c r="A50" s="3" t="inlineStr">
         <is>
           <t>GABBY</t>
         </is>
       </c>
-      <c r="B50" t="n">
+      <c r="B50" s="4" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
+      <c r="A51" s="3" t="inlineStr">
         <is>
           <t>BREN</t>
         </is>
       </c>
-      <c r="B51" t="n">
+      <c r="B51" s="4" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
+      <c r="A52" s="3" t="inlineStr">
         <is>
           <t>JADE ARAGON</t>
         </is>
       </c>
-      <c r="B52" t="n">
+      <c r="B52" s="4" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
+      <c r="A53" s="3" t="inlineStr">
         <is>
           <t>DAYANA V</t>
         </is>
       </c>
-      <c r="B53" t="n">
+      <c r="B53" s="4" t="n">
         <v>28</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
+      <c r="A54" s="3" t="inlineStr">
         <is>
           <t>YOHANNY</t>
         </is>
       </c>
-      <c r="B54" t="n">
+      <c r="B54" s="4" t="n">
         <v>27</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
+      <c r="A55" s="3" t="inlineStr">
         <is>
           <t>ANAILETH</t>
         </is>
       </c>
-      <c r="B55" t="n">
+      <c r="B55" s="4" t="n">
         <v>27</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
+      <c r="A56" s="3" t="inlineStr">
         <is>
           <t>ARLIN</t>
         </is>
       </c>
-      <c r="B56" t="n">
+      <c r="B56" s="4" t="n">
         <v>27</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
+      <c r="A57" s="3" t="inlineStr">
         <is>
           <t>LAURIS ELIZABETH</t>
         </is>
       </c>
-      <c r="B57" t="n">
+      <c r="B57" s="4" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
+      <c r="A58" s="3" t="inlineStr">
         <is>
           <t>BRENDA</t>
         </is>
       </c>
-      <c r="B58" t="n">
+      <c r="B58" s="4" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
+      <c r="A59" s="3" t="inlineStr">
         <is>
           <t>KEYLA PEREZ</t>
         </is>
       </c>
-      <c r="B59" t="n">
+      <c r="B59" s="4" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
+      <c r="A60" s="3" t="inlineStr">
         <is>
           <t>FLOR CABRERA</t>
         </is>
       </c>
-      <c r="B60" t="n">
+      <c r="B60" s="4" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
+      <c r="A61" s="3" t="inlineStr">
         <is>
           <t>YULIANA</t>
         </is>
       </c>
-      <c r="B61" t="n">
+      <c r="B61" s="4" t="n">
         <v>22</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
+      <c r="A62" s="3" t="inlineStr">
         <is>
           <t>IDEY</t>
         </is>
       </c>
-      <c r="B62" t="n">
+      <c r="B62" s="4" t="n">
         <v>22</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr">
+      <c r="A63" s="3" t="inlineStr">
         <is>
           <t>BRIGITTE</t>
         </is>
       </c>
-      <c r="B63" t="n">
+      <c r="B63" s="4" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
+      <c r="A64" s="3" t="inlineStr">
         <is>
           <t>ISIS LOPEZ</t>
         </is>
       </c>
-      <c r="B64" t="n">
+      <c r="B64" s="4" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
+      <c r="A65" s="3" t="inlineStr">
         <is>
           <t>ISABEL</t>
         </is>
       </c>
-      <c r="B65" t="n">
+      <c r="B65" s="4" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr">
+      <c r="A66" s="3" t="inlineStr">
         <is>
           <t>SARAHI</t>
         </is>
       </c>
-      <c r="B66" t="n">
+      <c r="B66" s="4" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr">
+      <c r="A67" s="3" t="inlineStr">
         <is>
           <t>CRISTY</t>
         </is>
       </c>
-      <c r="B67" t="n">
+      <c r="B67" s="4" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
+      <c r="A68" s="3" t="inlineStr">
         <is>
           <t>YAHAIRA BAUTISTA</t>
         </is>
       </c>
-      <c r="B68" t="n">
+      <c r="B68" s="4" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
+      <c r="A69" s="3" t="inlineStr">
         <is>
           <t>VAKITA</t>
         </is>
       </c>
-      <c r="B69" t="n">
+      <c r="B69" s="4" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
+      <c r="A70" s="3" t="inlineStr">
         <is>
           <t>HIJA DEL REY</t>
         </is>
       </c>
-      <c r="B70" t="n">
+      <c r="B70" s="4" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
+      <c r="A71" s="3" t="inlineStr">
         <is>
           <t>GABRIELA ALEJANDRA</t>
         </is>
       </c>
-      <c r="B71" t="n">
+      <c r="B71" s="4" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr">
+      <c r="A72" s="3" t="inlineStr">
         <is>
           <t>MILE</t>
         </is>
       </c>
-      <c r="B72" t="n">
+      <c r="B72" s="4" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr">
+      <c r="A73" s="3" t="inlineStr">
         <is>
           <t>JESSICA HERNANDEZ</t>
         </is>
       </c>
-      <c r="B73" t="n">
+      <c r="B73" s="4" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr">
+      <c r="A74" s="3" t="inlineStr">
         <is>
           <t>SADY URBINA</t>
         </is>
       </c>
-      <c r="B74" t="n">
+      <c r="B74" s="4" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr">
+      <c r="A75" s="3" t="inlineStr">
         <is>
           <t>YESSICA</t>
         </is>
       </c>
-      <c r="B75" t="n">
+      <c r="B75" s="4" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr">
+      <c r="A76" s="3" t="inlineStr">
         <is>
           <t>ESMIRNA</t>
         </is>
       </c>
-      <c r="B76" t="n">
+      <c r="B76" s="4" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="inlineStr">
+      <c r="A77" s="3" t="inlineStr">
         <is>
           <t>MARJORIE DILONE</t>
         </is>
       </c>
-      <c r="B77" t="n">
+      <c r="B77" s="4" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr">
+      <c r="A78" s="3" t="inlineStr">
         <is>
           <t>NATH CEDE</t>
         </is>
       </c>
-      <c r="B78" t="n">
+      <c r="B78" s="4" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="inlineStr">
+      <c r="A79" s="3" t="inlineStr">
         <is>
           <t>MICHELLE</t>
         </is>
       </c>
-      <c r="B79" t="n">
+      <c r="B79" s="4" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr">
+      <c r="A80" s="3" t="inlineStr">
         <is>
           <t>ERI V</t>
         </is>
       </c>
-      <c r="B80" t="n">
+      <c r="B80" s="4" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr">
+      <c r="A81" s="3" t="inlineStr">
         <is>
           <t>KARLA PINTO</t>
         </is>
       </c>
-      <c r="B81" t="n">
+      <c r="B81" s="4" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="inlineStr">
+      <c r="A82" s="3" t="inlineStr">
         <is>
           <t>KAMILL GROSS</t>
         </is>
       </c>
-      <c r="B82" t="n">
+      <c r="B82" s="4" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="inlineStr">
+      <c r="A83" s="3" t="inlineStr">
         <is>
           <t>YANI</t>
         </is>
       </c>
-      <c r="B83" t="n">
+      <c r="B83" s="4" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="inlineStr">
+      <c r="A84" s="3" t="inlineStr">
         <is>
           <t>TB</t>
         </is>
       </c>
-      <c r="B84" t="n">
+      <c r="B84" s="4" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="inlineStr">
+      <c r="A85" s="3" t="inlineStr">
         <is>
           <t>MARIA FERNANDA</t>
         </is>
       </c>
-      <c r="B85" t="n">
+      <c r="B85" s="4" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="inlineStr">
+      <c r="A86" s="3" t="inlineStr">
         <is>
           <t>KRISMAR</t>
         </is>
       </c>
-      <c r="B86" t="n">
+      <c r="B86" s="4" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="inlineStr">
+      <c r="A87" s="3" t="inlineStr">
         <is>
           <t>JESSICA PEGUERO</t>
         </is>
       </c>
-      <c r="B87" t="n">
+      <c r="B87" s="4" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="inlineStr">
+      <c r="A88" s="3" t="inlineStr">
         <is>
           <t>MARISOL</t>
         </is>
       </c>
-      <c r="B88" t="n">
+      <c r="B88" s="4" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="inlineStr">
+      <c r="A89" s="3" t="inlineStr">
         <is>
           <t>HEYSY</t>
         </is>
       </c>
-      <c r="B89" t="n">
+      <c r="B89" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="inlineStr">
+      <c r="A90" s="3" t="inlineStr">
         <is>
           <t>EVE</t>
         </is>
       </c>
-      <c r="B90" t="n">
+      <c r="B90" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="inlineStr">
+      <c r="A91" s="3" t="inlineStr">
         <is>
           <t>RITA</t>
         </is>
       </c>
-      <c r="B91" t="n">
+      <c r="B91" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="inlineStr">
+      <c r="A92" s="3" t="inlineStr">
         <is>
           <t>ROSI</t>
         </is>
       </c>
-      <c r="B92" t="n">
+      <c r="B92" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="inlineStr">
+      <c r="A93" s="3" t="inlineStr">
         <is>
           <t>ALE</t>
         </is>
       </c>
-      <c r="B93" t="n">
+      <c r="B93" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="inlineStr">
+      <c r="A94" s="3" t="inlineStr">
         <is>
           <t>MARIOBI CASTRO</t>
         </is>
       </c>
-      <c r="B94" t="n">
+      <c r="B94" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="inlineStr">
+      <c r="A95" s="3" t="inlineStr">
         <is>
           <t>MARIA JOSE</t>
         </is>
       </c>
-      <c r="B95" t="n">
+      <c r="B95" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="96">
-      <c r="A96" t="inlineStr">
+      <c r="A96" s="3" t="inlineStr">
         <is>
           <t>BERE</t>
         </is>
       </c>
-      <c r="B96" t="n">
+      <c r="B96" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="inlineStr">
+      <c r="A97" s="3" t="inlineStr">
         <is>
           <t>MAYVI</t>
         </is>
       </c>
-      <c r="B97" t="n">
+      <c r="B97" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="inlineStr">
+      <c r="A98" s="3" t="inlineStr">
         <is>
           <t>PRISCILA</t>
         </is>
       </c>
-      <c r="B98" t="n">
+      <c r="B98" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="inlineStr">
+      <c r="A99" s="3" t="inlineStr">
         <is>
           <t>YAMILETH</t>
         </is>
       </c>
-      <c r="B99" t="n">
+      <c r="B99" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="inlineStr">
+      <c r="A100" s="3" t="inlineStr">
         <is>
           <t>KEDMY A SANLATE V</t>
         </is>
       </c>
-      <c r="B100" t="n">
+      <c r="B100" s="4" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="inlineStr">
+      <c r="A101" s="3" t="inlineStr">
         <is>
           <t>EDIXIA MARADIAGA</t>
         </is>
       </c>
-      <c r="B101" t="n">
+      <c r="B101" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="inlineStr">
+      <c r="A102" s="3" t="inlineStr">
         <is>
           <t>BAUTISTA</t>
         </is>
       </c>
-      <c r="B102" t="n">
+      <c r="B102" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="inlineStr">
+      <c r="A103" s="3" t="inlineStr">
         <is>
           <t>AURY BEATO</t>
         </is>
       </c>
-      <c r="B103" t="n">
+      <c r="B103" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="inlineStr">
+      <c r="A104" s="3" t="inlineStr">
         <is>
           <t>MARY TORRES</t>
         </is>
       </c>
-      <c r="B104" t="n">
+      <c r="B104" s="4" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>